<commit_message>
more work on presentation
</commit_message>
<xml_diff>
--- a/data/cleaned_data/2013_TX.xlsx
+++ b/data/cleaned_data/2013_TX.xlsx
@@ -2157,7 +2157,7 @@
         <v>262</v>
       </c>
       <c r="D2">
-        <v>203</v>
+        <v>415</v>
       </c>
       <c r="E2" t="s">
         <v>308</v>
@@ -2183,7 +2183,7 @@
         <v>263</v>
       </c>
       <c r="D3">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
         <v>309</v>
@@ -2209,7 +2209,7 @@
         <v>264</v>
       </c>
       <c r="D4">
-        <v>532</v>
+        <v>863</v>
       </c>
       <c r="E4" t="s">
         <v>310</v>
@@ -2235,7 +2235,7 @@
         <v>265</v>
       </c>
       <c r="D5">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
         <v>311</v>
@@ -2261,7 +2261,7 @@
         <v>266</v>
       </c>
       <c r="D6">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>312</v>
@@ -2287,7 +2287,7 @@
         <v>267</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>313</v>
@@ -2313,7 +2313,7 @@
         <v>266</v>
       </c>
       <c r="D8">
-        <v>222</v>
+        <v>398</v>
       </c>
       <c r="E8" t="s">
         <v>314</v>
@@ -2339,7 +2339,7 @@
         <v>267</v>
       </c>
       <c r="D9">
-        <v>123</v>
+        <v>188</v>
       </c>
       <c r="E9" t="s">
         <v>315</v>
@@ -2365,7 +2365,7 @@
         <v>268</v>
       </c>
       <c r="D10">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>316</v>
@@ -2385,7 +2385,7 @@
         <v>269</v>
       </c>
       <c r="D11">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="E11" t="s">
         <v>317</v>
@@ -2411,7 +2411,7 @@
         <v>270</v>
       </c>
       <c r="D12">
-        <v>390</v>
+        <v>595</v>
       </c>
       <c r="E12" t="s">
         <v>318</v>
@@ -2437,7 +2437,7 @@
         <v>266</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
         <v>319</v>
@@ -2457,7 +2457,7 @@
         <v>271</v>
       </c>
       <c r="D14">
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="E14" t="s">
         <v>320</v>
@@ -2483,7 +2483,7 @@
         <v>272</v>
       </c>
       <c r="D15">
-        <v>1635</v>
+        <v>2727</v>
       </c>
       <c r="E15" t="s">
         <v>321</v>
@@ -2509,7 +2509,7 @@
         <v>273</v>
       </c>
       <c r="D16">
-        <v>14998</v>
+        <v>19612</v>
       </c>
       <c r="E16" t="s">
         <v>322</v>
@@ -2535,7 +2535,7 @@
         <v>274</v>
       </c>
       <c r="D17">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
         <v>323</v>
@@ -2555,7 +2555,7 @@
         <v>275</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
         <v>276</v>
@@ -2575,7 +2575,7 @@
         <v>274</v>
       </c>
       <c r="D19">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
         <v>324</v>
@@ -2595,7 +2595,7 @@
         <v>276</v>
       </c>
       <c r="D20">
-        <v>670</v>
+        <v>1060</v>
       </c>
       <c r="E20" t="s">
         <v>325</v>
@@ -2621,7 +2621,7 @@
         <v>277</v>
       </c>
       <c r="D21">
-        <v>1232</v>
+        <v>1880</v>
       </c>
       <c r="E21" t="s">
         <v>326</v>
@@ -2647,7 +2647,7 @@
         <v>278</v>
       </c>
       <c r="D22">
-        <v>971</v>
+        <v>1770</v>
       </c>
       <c r="E22" t="s">
         <v>327</v>
@@ -2673,7 +2673,7 @@
         <v>271</v>
       </c>
       <c r="D23">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
         <v>328</v>
@@ -2693,7 +2693,7 @@
         <v>279</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
         <v>270</v>
@@ -2713,7 +2713,7 @@
         <v>280</v>
       </c>
       <c r="D25">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
         <v>329</v>
@@ -2733,7 +2733,7 @@
         <v>268</v>
       </c>
       <c r="D26">
-        <v>179</v>
+        <v>248</v>
       </c>
       <c r="E26" t="s">
         <v>330</v>
@@ -2759,7 +2759,7 @@
         <v>271</v>
       </c>
       <c r="D27">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="E27" t="s">
         <v>331</v>
@@ -2785,7 +2785,7 @@
         <v>280</v>
       </c>
       <c r="D28">
-        <v>211</v>
+        <v>357</v>
       </c>
       <c r="E28" t="s">
         <v>332</v>
@@ -2805,7 +2805,7 @@
         <v>265</v>
       </c>
       <c r="D29">
-        <v>195</v>
+        <v>294</v>
       </c>
       <c r="E29" t="s">
         <v>333</v>
@@ -2831,7 +2831,7 @@
         <v>266</v>
       </c>
       <c r="D30">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
         <v>334</v>
@@ -2857,7 +2857,7 @@
         <v>263</v>
       </c>
       <c r="D31">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s">
         <v>335</v>
@@ -2883,7 +2883,7 @@
         <v>281</v>
       </c>
       <c r="D32">
-        <v>2305</v>
+        <v>3272</v>
       </c>
       <c r="E32" t="s">
         <v>336</v>
@@ -2909,7 +2909,7 @@
         <v>268</v>
       </c>
       <c r="D33">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
         <v>337</v>
@@ -2935,7 +2935,7 @@
         <v>275</v>
       </c>
       <c r="D34">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E34" t="s">
         <v>338</v>
@@ -2961,7 +2961,7 @@
         <v>266</v>
       </c>
       <c r="D35">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="E35" t="s">
         <v>339</v>
@@ -2981,7 +2981,7 @@
         <v>268</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
         <v>340</v>
@@ -3001,7 +3001,7 @@
         <v>282</v>
       </c>
       <c r="D37">
-        <v>269</v>
+        <v>432</v>
       </c>
       <c r="E37" t="s">
         <v>341</v>
@@ -3027,7 +3027,7 @@
         <v>278</v>
       </c>
       <c r="D38">
-        <v>185</v>
+        <v>335</v>
       </c>
       <c r="E38" t="s">
         <v>342</v>
@@ -3053,7 +3053,7 @@
         <v>268</v>
       </c>
       <c r="D39">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E39" t="s">
         <v>343</v>
@@ -3073,7 +3073,7 @@
         <v>267</v>
       </c>
       <c r="D40">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
         <v>344</v>
@@ -3099,7 +3099,7 @@
         <v>279</v>
       </c>
       <c r="D41">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E41" t="s">
         <v>305</v>
@@ -3119,7 +3119,7 @@
         <v>275</v>
       </c>
       <c r="D42">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
         <v>345</v>
@@ -3139,7 +3139,7 @@
         <v>275</v>
       </c>
       <c r="D43">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
         <v>346</v>
@@ -3159,7 +3159,7 @@
         <v>283</v>
       </c>
       <c r="D44">
-        <v>3253</v>
+        <v>5193</v>
       </c>
       <c r="E44" t="s">
         <v>347</v>
@@ -3185,7 +3185,7 @@
         <v>279</v>
       </c>
       <c r="D45">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
         <v>303</v>
@@ -3205,7 +3205,7 @@
         <v>278</v>
       </c>
       <c r="D46">
-        <v>94</v>
+        <v>194</v>
       </c>
       <c r="E46" t="s">
         <v>348</v>
@@ -3225,7 +3225,7 @@
         <v>284</v>
       </c>
       <c r="D47">
-        <v>632</v>
+        <v>978</v>
       </c>
       <c r="E47" t="s">
         <v>349</v>
@@ -3251,7 +3251,7 @@
         <v>274</v>
       </c>
       <c r="D48">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="E48" t="s">
         <v>350</v>
@@ -3271,7 +3271,7 @@
         <v>265</v>
       </c>
       <c r="D49">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E49" t="s">
         <v>305</v>
@@ -3291,7 +3291,7 @@
         <v>271</v>
       </c>
       <c r="D50">
-        <v>186</v>
+        <v>310</v>
       </c>
       <c r="E50" t="s">
         <v>351</v>
@@ -3317,7 +3317,7 @@
         <v>266</v>
       </c>
       <c r="D51">
-        <v>315</v>
+        <v>544</v>
       </c>
       <c r="E51" t="s">
         <v>352</v>
@@ -3343,7 +3343,7 @@
         <v>279</v>
       </c>
       <c r="D52">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E52" t="s">
         <v>291</v>
@@ -3363,7 +3363,7 @@
         <v>268</v>
       </c>
       <c r="D53">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E53" t="s">
         <v>319</v>
@@ -3383,7 +3383,7 @@
         <v>274</v>
       </c>
       <c r="D54">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="E54" t="s">
         <v>353</v>
@@ -3403,7 +3403,7 @@
         <v>279</v>
       </c>
       <c r="D55">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E55" t="s">
         <v>354</v>
@@ -3429,7 +3429,7 @@
         <v>268</v>
       </c>
       <c r="D56">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="E56" t="s">
         <v>355</v>
@@ -3449,7 +3449,7 @@
         <v>275</v>
       </c>
       <c r="D57">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E57" t="s">
         <v>356</v>
@@ -3469,7 +3469,7 @@
         <v>285</v>
       </c>
       <c r="D58">
-        <v>17877</v>
+        <v>24950</v>
       </c>
       <c r="E58" t="s">
         <v>357</v>
@@ -3495,7 +3495,7 @@
         <v>265</v>
       </c>
       <c r="D59">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="E59" t="s">
         <v>358</v>
@@ -3521,7 +3521,7 @@
         <v>268</v>
       </c>
       <c r="D60">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="E60" t="s">
         <v>359</v>
@@ -3547,7 +3547,7 @@
         <v>268</v>
       </c>
       <c r="D61">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E61" t="s">
         <v>286</v>
@@ -3567,7 +3567,7 @@
         <v>281</v>
       </c>
       <c r="D62">
-        <v>2754</v>
+        <v>4199</v>
       </c>
       <c r="E62" t="s">
         <v>360</v>
@@ -3593,7 +3593,7 @@
         <v>262</v>
       </c>
       <c r="D63">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="E63" t="s">
         <v>361</v>
@@ -3613,7 +3613,7 @@
         <v>279</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E64" t="s">
         <v>293</v>
@@ -3633,7 +3633,7 @@
         <v>269</v>
       </c>
       <c r="D65">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="E65" t="s">
         <v>362</v>
@@ -3653,7 +3653,7 @@
         <v>275</v>
       </c>
       <c r="D66">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E66" t="s">
         <v>363</v>
@@ -3673,7 +3673,7 @@
         <v>274</v>
       </c>
       <c r="D67">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="E67" t="s">
         <v>356</v>
@@ -3699,7 +3699,7 @@
         <v>280</v>
       </c>
       <c r="D68">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="E68" t="s">
         <v>364</v>
@@ -3719,7 +3719,7 @@
         <v>286</v>
       </c>
       <c r="D69">
-        <v>1179</v>
+        <v>1901</v>
       </c>
       <c r="E69" t="s">
         <v>365</v>
@@ -3745,7 +3745,7 @@
         <v>279</v>
       </c>
       <c r="D70">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E70" t="s">
         <v>366</v>
@@ -3765,7 +3765,7 @@
         <v>264</v>
       </c>
       <c r="D71">
-        <v>596</v>
+        <v>966</v>
       </c>
       <c r="E71" t="s">
         <v>367</v>
@@ -3791,7 +3791,7 @@
         <v>286</v>
       </c>
       <c r="D72">
-        <v>4715</v>
+        <v>6785</v>
       </c>
       <c r="E72" t="s">
         <v>368</v>
@@ -3817,7 +3817,7 @@
         <v>269</v>
       </c>
       <c r="D73">
-        <v>131</v>
+        <v>251</v>
       </c>
       <c r="E73" t="s">
         <v>369</v>
@@ -3843,7 +3843,7 @@
         <v>280</v>
       </c>
       <c r="D74">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="E74" t="s">
         <v>370</v>
@@ -3869,7 +3869,7 @@
         <v>267</v>
       </c>
       <c r="D75">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="E75" t="s">
         <v>371</v>
@@ -3895,7 +3895,7 @@
         <v>287</v>
       </c>
       <c r="D76">
-        <v>140</v>
+        <v>237</v>
       </c>
       <c r="E76" t="s">
         <v>372</v>
@@ -3915,7 +3915,7 @@
         <v>275</v>
       </c>
       <c r="D77">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E77" t="s">
         <v>373</v>
@@ -3935,7 +3935,7 @@
         <v>268</v>
       </c>
       <c r="D78">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E78" t="s">
         <v>374</v>
@@ -3955,7 +3955,7 @@
         <v>268</v>
       </c>
       <c r="D79">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E79" t="s">
         <v>263</v>
@@ -3975,7 +3975,7 @@
         <v>288</v>
       </c>
       <c r="D80">
-        <v>1989</v>
+        <v>2954</v>
       </c>
       <c r="E80" t="s">
         <v>375</v>
@@ -4001,7 +4001,7 @@
         <v>268</v>
       </c>
       <c r="D81">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E81" t="s">
         <v>376</v>
@@ -4021,7 +4021,7 @@
         <v>274</v>
       </c>
       <c r="D82">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="E82" t="s">
         <v>377</v>
@@ -4041,7 +4041,7 @@
         <v>266</v>
       </c>
       <c r="D83">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="E83" t="s">
         <v>378</v>
@@ -4067,7 +4067,7 @@
         <v>287</v>
       </c>
       <c r="D84">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="E84" t="s">
         <v>379</v>
@@ -4087,7 +4087,7 @@
         <v>289</v>
       </c>
       <c r="D85">
-        <v>1436</v>
+        <v>2065</v>
       </c>
       <c r="E85" t="s">
         <v>380</v>
@@ -4113,7 +4113,7 @@
         <v>275</v>
       </c>
       <c r="D86">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E86" t="s">
         <v>381</v>
@@ -4133,7 +4133,7 @@
         <v>267</v>
       </c>
       <c r="D87">
-        <v>117</v>
+        <v>219</v>
       </c>
       <c r="E87" t="s">
         <v>382</v>
@@ -4159,7 +4159,7 @@
         <v>265</v>
       </c>
       <c r="D88">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="E88" t="s">
         <v>383</v>
@@ -4179,7 +4179,7 @@
         <v>271</v>
       </c>
       <c r="D89">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E89" t="s">
         <v>350</v>
@@ -4205,7 +4205,7 @@
         <v>287</v>
       </c>
       <c r="D90">
-        <v>143</v>
+        <v>243</v>
       </c>
       <c r="E90" t="s">
         <v>384</v>
@@ -4225,7 +4225,7 @@
         <v>271</v>
       </c>
       <c r="D91">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="E91" t="s">
         <v>385</v>
@@ -4251,7 +4251,7 @@
         <v>290</v>
       </c>
       <c r="D92">
-        <v>496</v>
+        <v>839</v>
       </c>
       <c r="E92" t="s">
         <v>386</v>
@@ -4277,7 +4277,7 @@
         <v>284</v>
       </c>
       <c r="D93">
-        <v>1526</v>
+        <v>1985</v>
       </c>
       <c r="E93" t="s">
         <v>387</v>
@@ -4303,7 +4303,7 @@
         <v>269</v>
       </c>
       <c r="D94">
-        <v>183</v>
+        <v>322</v>
       </c>
       <c r="E94" t="s">
         <v>388</v>
@@ -4323,7 +4323,7 @@
         <v>291</v>
       </c>
       <c r="D95">
-        <v>566</v>
+        <v>948</v>
       </c>
       <c r="E95" t="s">
         <v>389</v>
@@ -4349,7 +4349,7 @@
         <v>275</v>
       </c>
       <c r="D96">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="E96" t="s">
         <v>390</v>
@@ -4375,7 +4375,7 @@
         <v>271</v>
       </c>
       <c r="D97">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E97" t="s">
         <v>391</v>
@@ -4395,7 +4395,7 @@
         <v>265</v>
       </c>
       <c r="D98">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E98" t="s">
         <v>392</v>
@@ -4415,7 +4415,7 @@
         <v>268</v>
       </c>
       <c r="D99">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E99" t="s">
         <v>281</v>
@@ -4435,7 +4435,7 @@
         <v>268</v>
       </c>
       <c r="D100">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E100" t="s">
         <v>393</v>
@@ -4455,7 +4455,7 @@
         <v>287</v>
       </c>
       <c r="D101">
-        <v>221</v>
+        <v>387</v>
       </c>
       <c r="E101" t="s">
         <v>394</v>
@@ -4481,7 +4481,7 @@
         <v>292</v>
       </c>
       <c r="D102">
-        <v>31828</v>
+        <v>41745</v>
       </c>
       <c r="E102" t="s">
         <v>395</v>
@@ -4507,7 +4507,7 @@
         <v>293</v>
       </c>
       <c r="D103">
-        <v>488</v>
+        <v>704</v>
       </c>
       <c r="E103" t="s">
         <v>396</v>
@@ -4533,7 +4533,7 @@
         <v>265</v>
       </c>
       <c r="D104">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E104" t="s">
         <v>397</v>
@@ -4553,7 +4553,7 @@
         <v>271</v>
       </c>
       <c r="D105">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E105" t="s">
         <v>398</v>
@@ -4573,7 +4573,7 @@
         <v>294</v>
       </c>
       <c r="D106">
-        <v>739</v>
+        <v>1247</v>
       </c>
       <c r="E106" t="s">
         <v>399</v>
@@ -4599,7 +4599,7 @@
         <v>275</v>
       </c>
       <c r="D107">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E107" t="s">
         <v>355</v>
@@ -4619,7 +4619,7 @@
         <v>263</v>
       </c>
       <c r="D108">
-        <v>414</v>
+        <v>618</v>
       </c>
       <c r="E108" t="s">
         <v>400</v>
@@ -4645,7 +4645,7 @@
         <v>295</v>
       </c>
       <c r="D109">
-        <v>6240</v>
+        <v>8182</v>
       </c>
       <c r="E109" t="s">
         <v>401</v>
@@ -4671,7 +4671,7 @@
         <v>291</v>
       </c>
       <c r="D110">
-        <v>197</v>
+        <v>316</v>
       </c>
       <c r="E110" t="s">
         <v>402</v>
@@ -4691,7 +4691,7 @@
         <v>267</v>
       </c>
       <c r="D111">
-        <v>112</v>
+        <v>187</v>
       </c>
       <c r="E111" t="s">
         <v>403</v>
@@ -4717,7 +4717,7 @@
         <v>274</v>
       </c>
       <c r="D112">
-        <v>200</v>
+        <v>321</v>
       </c>
       <c r="E112" t="s">
         <v>404</v>
@@ -4743,7 +4743,7 @@
         <v>266</v>
       </c>
       <c r="D113">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="E113" t="s">
         <v>405</v>
@@ -4769,7 +4769,7 @@
         <v>280</v>
       </c>
       <c r="D114">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="E114" t="s">
         <v>317</v>
@@ -4789,7 +4789,7 @@
         <v>263</v>
       </c>
       <c r="D115">
-        <v>154</v>
+        <v>292</v>
       </c>
       <c r="E115" t="s">
         <v>406</v>
@@ -4815,7 +4815,7 @@
         <v>296</v>
       </c>
       <c r="D116">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E116" t="s">
         <v>407</v>
@@ -4841,7 +4841,7 @@
         <v>278</v>
       </c>
       <c r="D117">
-        <v>384</v>
+        <v>553</v>
       </c>
       <c r="E117" t="s">
         <v>408</v>
@@ -4867,7 +4867,7 @@
         <v>267</v>
       </c>
       <c r="D118">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="E118" t="s">
         <v>409</v>
@@ -4893,7 +4893,7 @@
         <v>268</v>
       </c>
       <c r="D119">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="E119" t="s">
         <v>373</v>
@@ -4919,7 +4919,7 @@
         <v>271</v>
       </c>
       <c r="D120">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E120" t="s">
         <v>346</v>
@@ -4939,7 +4939,7 @@
         <v>267</v>
       </c>
       <c r="D121">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="E121" t="s">
         <v>410</v>
@@ -4959,7 +4959,7 @@
         <v>280</v>
       </c>
       <c r="D122">
-        <v>169</v>
+        <v>243</v>
       </c>
       <c r="E122" t="s">
         <v>411</v>
@@ -4979,7 +4979,7 @@
         <v>271</v>
       </c>
       <c r="D123">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E123" t="s">
         <v>363</v>
@@ -4999,7 +4999,7 @@
         <v>293</v>
       </c>
       <c r="D124">
-        <v>2082</v>
+        <v>2912</v>
       </c>
       <c r="E124" t="s">
         <v>412</v>
@@ -5025,7 +5025,7 @@
         <v>275</v>
       </c>
       <c r="D125">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E125" t="s">
         <v>374</v>
@@ -5045,7 +5045,7 @@
         <v>296</v>
       </c>
       <c r="D126">
-        <v>438</v>
+        <v>576</v>
       </c>
       <c r="E126" t="s">
         <v>413</v>
@@ -5071,7 +5071,7 @@
         <v>264</v>
       </c>
       <c r="D127">
-        <v>559</v>
+        <v>965</v>
       </c>
       <c r="E127" t="s">
         <v>414</v>
@@ -5097,7 +5097,7 @@
         <v>266</v>
       </c>
       <c r="D128">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E128" t="s">
         <v>415</v>
@@ -5123,7 +5123,7 @@
         <v>287</v>
       </c>
       <c r="D129">
-        <v>117</v>
+        <v>203</v>
       </c>
       <c r="E129" t="s">
         <v>416</v>
@@ -5143,7 +5143,7 @@
         <v>263</v>
       </c>
       <c r="D130">
-        <v>428</v>
+        <v>635</v>
       </c>
       <c r="E130" t="s">
         <v>417</v>
@@ -5169,7 +5169,7 @@
         <v>280</v>
       </c>
       <c r="D131">
-        <v>141</v>
+        <v>252</v>
       </c>
       <c r="E131" t="s">
         <v>418</v>
@@ -5195,7 +5195,7 @@
         <v>268</v>
       </c>
       <c r="D132">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E132" t="s">
         <v>391</v>
@@ -5221,7 +5221,7 @@
         <v>279</v>
       </c>
       <c r="D133">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E133" t="s">
         <v>270</v>
@@ -5241,7 +5241,7 @@
         <v>291</v>
       </c>
       <c r="D134">
-        <v>262</v>
+        <v>404</v>
       </c>
       <c r="E134" t="s">
         <v>419</v>
@@ -5267,7 +5267,7 @@
         <v>265</v>
       </c>
       <c r="D135">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E135" t="s">
         <v>420</v>
@@ -5287,7 +5287,7 @@
         <v>279</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E136" t="s">
         <v>293</v>
@@ -5307,7 +5307,7 @@
         <v>268</v>
       </c>
       <c r="D137">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E137" t="s">
         <v>421</v>
@@ -5327,7 +5327,7 @@
         <v>274</v>
       </c>
       <c r="D138">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="E138" t="s">
         <v>422</v>
@@ -5353,7 +5353,7 @@
         <v>275</v>
       </c>
       <c r="D139">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E139" t="s">
         <v>423</v>
@@ -5373,7 +5373,7 @@
         <v>266</v>
       </c>
       <c r="D140">
-        <v>248</v>
+        <v>407</v>
       </c>
       <c r="E140" t="s">
         <v>424</v>
@@ -5399,7 +5399,7 @@
         <v>280</v>
       </c>
       <c r="D141">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="E141" t="s">
         <v>425</v>
@@ -5419,7 +5419,7 @@
         <v>271</v>
       </c>
       <c r="D142">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E142" t="s">
         <v>426</v>
@@ -5445,7 +5445,7 @@
         <v>262</v>
       </c>
       <c r="D143">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="E143" t="s">
         <v>427</v>
@@ -5465,7 +5465,7 @@
         <v>265</v>
       </c>
       <c r="D144">
-        <v>82</v>
+        <v>133</v>
       </c>
       <c r="E144" t="s">
         <v>427</v>
@@ -5485,7 +5485,7 @@
         <v>280</v>
       </c>
       <c r="D145">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="E145" t="s">
         <v>428</v>
@@ -5505,7 +5505,7 @@
         <v>263</v>
       </c>
       <c r="D146">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="E146" t="s">
         <v>429</v>
@@ -5525,7 +5525,7 @@
         <v>294</v>
       </c>
       <c r="D147">
-        <v>409</v>
+        <v>603</v>
       </c>
       <c r="E147" t="s">
         <v>430</v>
@@ -5551,7 +5551,7 @@
         <v>265</v>
       </c>
       <c r="D148">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="E148" t="s">
         <v>431</v>
@@ -5571,7 +5571,7 @@
         <v>279</v>
       </c>
       <c r="D149">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E149" t="s">
         <v>293</v>
@@ -5591,7 +5591,7 @@
         <v>278</v>
       </c>
       <c r="D150">
-        <v>173</v>
+        <v>272</v>
       </c>
       <c r="E150" t="s">
         <v>432</v>
@@ -5611,7 +5611,7 @@
         <v>265</v>
       </c>
       <c r="D151">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="E151" t="s">
         <v>433</v>
@@ -5631,7 +5631,7 @@
         <v>279</v>
       </c>
       <c r="D152">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E152" t="s">
         <v>303</v>
@@ -5657,7 +5657,7 @@
         <v>297</v>
       </c>
       <c r="D153">
-        <v>3343</v>
+        <v>4157</v>
       </c>
       <c r="E153" t="s">
         <v>434</v>
@@ -5683,7 +5683,7 @@
         <v>275</v>
       </c>
       <c r="D154">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E154" t="s">
         <v>343</v>
@@ -5709,7 +5709,7 @@
         <v>266</v>
       </c>
       <c r="D155">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="E155" t="s">
         <v>435</v>
@@ -5729,7 +5729,7 @@
         <v>266</v>
       </c>
       <c r="D156">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E156" t="s">
         <v>436</v>
@@ -5749,7 +5749,7 @@
         <v>271</v>
       </c>
       <c r="D157">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="E157" t="s">
         <v>324</v>
@@ -5775,7 +5775,7 @@
         <v>268</v>
       </c>
       <c r="D158">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E158" t="s">
         <v>437</v>
@@ -5795,7 +5795,7 @@
         <v>280</v>
       </c>
       <c r="D159">
-        <v>209</v>
+        <v>286</v>
       </c>
       <c r="E159" t="s">
         <v>438</v>
@@ -5821,7 +5821,7 @@
         <v>274</v>
       </c>
       <c r="D160">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="E160" t="s">
         <v>439</v>
@@ -5847,7 +5847,7 @@
         <v>279</v>
       </c>
       <c r="D161">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="E161" t="s">
         <v>440</v>
@@ -5867,7 +5867,7 @@
         <v>298</v>
       </c>
       <c r="D162">
-        <v>1702</v>
+        <v>2669</v>
       </c>
       <c r="E162" t="s">
         <v>441</v>
@@ -5893,7 +5893,7 @@
         <v>279</v>
       </c>
       <c r="D163">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E163" t="s">
         <v>442</v>
@@ -5913,7 +5913,7 @@
         <v>287</v>
       </c>
       <c r="D164">
-        <v>172</v>
+        <v>298</v>
       </c>
       <c r="E164" t="s">
         <v>443</v>
@@ -5939,7 +5939,7 @@
         <v>275</v>
       </c>
       <c r="D165">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E165" t="s">
         <v>345</v>
@@ -5959,7 +5959,7 @@
         <v>299</v>
       </c>
       <c r="D166">
-        <v>931</v>
+        <v>1421</v>
       </c>
       <c r="E166" t="s">
         <v>444</v>
@@ -5985,7 +5985,7 @@
         <v>265</v>
       </c>
       <c r="D167">
-        <v>96</v>
+        <v>173</v>
       </c>
       <c r="E167" t="s">
         <v>445</v>
@@ -6005,7 +6005,7 @@
         <v>275</v>
       </c>
       <c r="D168">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E168" t="s">
         <v>446</v>
@@ -6025,7 +6025,7 @@
         <v>275</v>
       </c>
       <c r="D169">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E169" t="s">
         <v>447</v>
@@ -6045,7 +6045,7 @@
         <v>271</v>
       </c>
       <c r="D170">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="E170" t="s">
         <v>448</v>
@@ -6065,7 +6065,7 @@
         <v>300</v>
       </c>
       <c r="D171">
-        <v>2364</v>
+        <v>3566</v>
       </c>
       <c r="E171" t="s">
         <v>449</v>
@@ -6091,7 +6091,7 @@
         <v>301</v>
       </c>
       <c r="D172">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="E172" t="s">
         <v>450</v>
@@ -6117,7 +6117,7 @@
         <v>268</v>
       </c>
       <c r="D173">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="E173" t="s">
         <v>324</v>
@@ -6137,7 +6137,7 @@
         <v>275</v>
       </c>
       <c r="D174">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E174" t="s">
         <v>276</v>
@@ -6157,7 +6157,7 @@
         <v>291</v>
       </c>
       <c r="D175">
-        <v>414</v>
+        <v>575</v>
       </c>
       <c r="E175" t="s">
         <v>451</v>
@@ -6183,7 +6183,7 @@
         <v>282</v>
       </c>
       <c r="D176">
-        <v>265</v>
+        <v>418</v>
       </c>
       <c r="E176" t="s">
         <v>452</v>
@@ -6209,7 +6209,7 @@
         <v>268</v>
       </c>
       <c r="D177">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E177" t="s">
         <v>453</v>
@@ -6229,7 +6229,7 @@
         <v>269</v>
       </c>
       <c r="D178">
-        <v>103</v>
+        <v>179</v>
       </c>
       <c r="E178" t="s">
         <v>454</v>
@@ -6255,7 +6255,7 @@
         <v>302</v>
       </c>
       <c r="D179">
-        <v>2568</v>
+        <v>3778</v>
       </c>
       <c r="E179" t="s">
         <v>455</v>
@@ -6281,7 +6281,7 @@
         <v>265</v>
       </c>
       <c r="D180">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E180" t="s">
         <v>350</v>
@@ -6301,7 +6301,7 @@
         <v>266</v>
       </c>
       <c r="D181">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="E181" t="s">
         <v>392</v>
@@ -6327,7 +6327,7 @@
         <v>282</v>
       </c>
       <c r="D182">
-        <v>439</v>
+        <v>738</v>
       </c>
       <c r="E182" t="s">
         <v>456</v>
@@ -6353,7 +6353,7 @@
         <v>287</v>
       </c>
       <c r="D183">
-        <v>72</v>
+        <v>198</v>
       </c>
       <c r="E183" t="s">
         <v>457</v>
@@ -6379,7 +6379,7 @@
         <v>287</v>
       </c>
       <c r="D184">
-        <v>151</v>
+        <v>207</v>
       </c>
       <c r="E184" t="s">
         <v>458</v>
@@ -6399,7 +6399,7 @@
         <v>303</v>
       </c>
       <c r="D185">
-        <v>461</v>
+        <v>787</v>
       </c>
       <c r="E185" t="s">
         <v>459</v>
@@ -6425,7 +6425,7 @@
         <v>275</v>
       </c>
       <c r="D186">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E186" t="s">
         <v>381</v>
@@ -6445,7 +6445,7 @@
         <v>266</v>
       </c>
       <c r="D187">
-        <v>109</v>
+        <v>215</v>
       </c>
       <c r="E187" t="s">
         <v>460</v>
@@ -6465,7 +6465,7 @@
         <v>263</v>
       </c>
       <c r="D188">
-        <v>225</v>
+        <v>387</v>
       </c>
       <c r="E188" t="s">
         <v>461</v>
@@ -6485,7 +6485,7 @@
         <v>297</v>
       </c>
       <c r="D189">
-        <v>922</v>
+        <v>1341</v>
       </c>
       <c r="E189" t="s">
         <v>462</v>
@@ -6511,7 +6511,7 @@
         <v>279</v>
       </c>
       <c r="D190">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E190" t="s">
         <v>463</v>
@@ -6531,7 +6531,7 @@
         <v>268</v>
       </c>
       <c r="D191">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="E191" t="s">
         <v>464</v>
@@ -6551,7 +6551,7 @@
         <v>282</v>
       </c>
       <c r="D192">
-        <v>496</v>
+        <v>725</v>
       </c>
       <c r="E192" t="s">
         <v>465</v>
@@ -6577,7 +6577,7 @@
         <v>265</v>
       </c>
       <c r="D193">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="E193" t="s">
         <v>466</v>
@@ -6597,7 +6597,7 @@
         <v>271</v>
       </c>
       <c r="D194">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E194" t="s">
         <v>467</v>
@@ -6617,7 +6617,7 @@
         <v>265</v>
       </c>
       <c r="D195">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="E195" t="s">
         <v>464</v>
@@ -6637,7 +6637,7 @@
         <v>301</v>
       </c>
       <c r="D196">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="E196" t="s">
         <v>468</v>
@@ -6663,7 +6663,7 @@
         <v>266</v>
       </c>
       <c r="D197">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="E197" t="s">
         <v>469</v>
@@ -6683,7 +6683,7 @@
         <v>275</v>
       </c>
       <c r="D198">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E198" t="s">
         <v>470</v>
@@ -6709,7 +6709,7 @@
         <v>266</v>
       </c>
       <c r="D199">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="E199" t="s">
         <v>471</v>
@@ -6735,7 +6735,7 @@
         <v>280</v>
       </c>
       <c r="D200">
-        <v>310</v>
+        <v>435</v>
       </c>
       <c r="E200" t="s">
         <v>472</v>
@@ -6761,7 +6761,7 @@
         <v>275</v>
       </c>
       <c r="D201">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E201" t="s">
         <v>473</v>
@@ -6781,7 +6781,7 @@
         <v>304</v>
       </c>
       <c r="D202">
-        <v>297</v>
+        <v>411</v>
       </c>
       <c r="E202" t="s">
         <v>474</v>
@@ -6807,7 +6807,7 @@
         <v>265</v>
       </c>
       <c r="D203">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="E203" t="s">
         <v>464</v>
@@ -6827,7 +6827,7 @@
         <v>267</v>
       </c>
       <c r="D204">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="E204" t="s">
         <v>475</v>
@@ -6847,7 +6847,7 @@
         <v>262</v>
       </c>
       <c r="D205">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="E205" t="s">
         <v>460</v>
@@ -6867,7 +6867,7 @@
         <v>263</v>
       </c>
       <c r="D206">
-        <v>357</v>
+        <v>521</v>
       </c>
       <c r="E206" t="s">
         <v>476</v>
@@ -6893,7 +6893,7 @@
         <v>271</v>
       </c>
       <c r="D207">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E207" t="s">
         <v>374</v>
@@ -6913,7 +6913,7 @@
         <v>274</v>
       </c>
       <c r="D208">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E208" t="s">
         <v>477</v>
@@ -6933,7 +6933,7 @@
         <v>265</v>
       </c>
       <c r="D209">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="E209" t="s">
         <v>478</v>
@@ -6959,7 +6959,7 @@
         <v>271</v>
       </c>
       <c r="D210">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E210" t="s">
         <v>286</v>
@@ -6979,7 +6979,7 @@
         <v>267</v>
       </c>
       <c r="D211">
-        <v>89</v>
+        <v>192</v>
       </c>
       <c r="E211" t="s">
         <v>479</v>
@@ -6999,7 +6999,7 @@
         <v>268</v>
       </c>
       <c r="D212">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E212" t="s">
         <v>480</v>
@@ -7019,7 +7019,7 @@
         <v>305</v>
       </c>
       <c r="D213">
-        <v>1626</v>
+        <v>2359</v>
       </c>
       <c r="E213" t="s">
         <v>481</v>
@@ -7045,7 +7045,7 @@
         <v>267</v>
       </c>
       <c r="D214">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="E214" t="s">
         <v>482</v>
@@ -7065,7 +7065,7 @@
         <v>282</v>
       </c>
       <c r="D215">
-        <v>271</v>
+        <v>452</v>
       </c>
       <c r="E215" t="s">
         <v>483</v>
@@ -7091,7 +7091,7 @@
         <v>268</v>
       </c>
       <c r="D216">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E216" t="s">
         <v>436</v>
@@ -7111,7 +7111,7 @@
         <v>279</v>
       </c>
       <c r="D217">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E217" t="s">
         <v>272</v>
@@ -7137,7 +7137,7 @@
         <v>271</v>
       </c>
       <c r="D218">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E218" t="s">
         <v>270</v>
@@ -7157,7 +7157,7 @@
         <v>267</v>
       </c>
       <c r="D219">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E219" t="s">
         <v>312</v>
@@ -7177,7 +7177,7 @@
         <v>268</v>
       </c>
       <c r="D220">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E220" t="s">
         <v>355</v>
@@ -7197,7 +7197,7 @@
         <v>306</v>
       </c>
       <c r="D221">
-        <v>10735</v>
+        <v>16029</v>
       </c>
       <c r="E221" t="s">
         <v>484</v>
@@ -7223,7 +7223,7 @@
         <v>270</v>
       </c>
       <c r="D222">
-        <v>1122</v>
+        <v>1669</v>
       </c>
       <c r="E222" t="s">
         <v>485</v>
@@ -7249,7 +7249,7 @@
         <v>275</v>
       </c>
       <c r="D223">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E223" t="s">
         <v>301</v>
@@ -7269,7 +7269,7 @@
         <v>266</v>
       </c>
       <c r="D224">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="E224" t="s">
         <v>407</v>
@@ -7289,7 +7289,7 @@
         <v>279</v>
       </c>
       <c r="D225">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E225" t="s">
         <v>303</v>
@@ -7309,7 +7309,7 @@
         <v>274</v>
       </c>
       <c r="D226">
-        <v>261</v>
+        <v>389</v>
       </c>
       <c r="E226" t="s">
         <v>486</v>
@@ -7335,7 +7335,7 @@
         <v>278</v>
       </c>
       <c r="D227">
-        <v>769</v>
+        <v>1192</v>
       </c>
       <c r="E227" t="s">
         <v>487</v>
@@ -7361,7 +7361,7 @@
         <v>307</v>
       </c>
       <c r="D228">
-        <v>6666</v>
+        <v>11849</v>
       </c>
       <c r="E228" t="s">
         <v>488</v>
@@ -7387,7 +7387,7 @@
         <v>274</v>
       </c>
       <c r="D229">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="E229" t="s">
         <v>489</v>
@@ -7407,7 +7407,7 @@
         <v>269</v>
       </c>
       <c r="D230">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="E230" t="s">
         <v>427</v>
@@ -7427,7 +7427,7 @@
         <v>274</v>
       </c>
       <c r="D231">
-        <v>188</v>
+        <v>313</v>
       </c>
       <c r="E231" t="s">
         <v>372</v>
@@ -7453,7 +7453,7 @@
         <v>275</v>
       </c>
       <c r="D232">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E232" t="s">
         <v>295</v>
@@ -7473,7 +7473,7 @@
         <v>280</v>
       </c>
       <c r="D233">
-        <v>196</v>
+        <v>277</v>
       </c>
       <c r="E233" t="s">
         <v>384</v>
@@ -7499,7 +7499,7 @@
         <v>280</v>
       </c>
       <c r="D234">
-        <v>231</v>
+        <v>311</v>
       </c>
       <c r="E234" t="s">
         <v>490</v>
@@ -7525,7 +7525,7 @@
         <v>293</v>
       </c>
       <c r="D235">
-        <v>303</v>
+        <v>461</v>
       </c>
       <c r="E235" t="s">
         <v>491</v>
@@ -7545,7 +7545,7 @@
         <v>282</v>
       </c>
       <c r="D236">
-        <v>405</v>
+        <v>824</v>
       </c>
       <c r="E236" t="s">
         <v>492</v>
@@ -7571,7 +7571,7 @@
         <v>287</v>
       </c>
       <c r="D237">
-        <v>351</v>
+        <v>529</v>
       </c>
       <c r="E237" t="s">
         <v>493</v>
@@ -7597,7 +7597,7 @@
         <v>264</v>
       </c>
       <c r="D238">
-        <v>296</v>
+        <v>403</v>
       </c>
       <c r="E238" t="s">
         <v>494</v>
@@ -7623,7 +7623,7 @@
         <v>267</v>
       </c>
       <c r="D239">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="E239" t="s">
         <v>495</v>
@@ -7643,7 +7643,7 @@
         <v>265</v>
       </c>
       <c r="D240">
-        <v>189</v>
+        <v>321</v>
       </c>
       <c r="E240" t="s">
         <v>308</v>
@@ -7669,7 +7669,7 @@
         <v>305</v>
       </c>
       <c r="D241">
-        <v>2150</v>
+        <v>3035</v>
       </c>
       <c r="E241" t="s">
         <v>496</v>
@@ -7695,7 +7695,7 @@
         <v>269</v>
       </c>
       <c r="D242">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="E242" t="s">
         <v>497</v>
@@ -7721,7 +7721,7 @@
         <v>268</v>
       </c>
       <c r="D243">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E243" t="s">
         <v>498</v>
@@ -7741,7 +7741,7 @@
         <v>278</v>
       </c>
       <c r="D244">
-        <v>405</v>
+        <v>692</v>
       </c>
       <c r="E244" t="s">
         <v>499</v>
@@ -7767,7 +7767,7 @@
         <v>268</v>
       </c>
       <c r="D245">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="E245" t="s">
         <v>500</v>
@@ -7793,7 +7793,7 @@
         <v>268</v>
       </c>
       <c r="D246">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="E246" t="s">
         <v>501</v>
@@ -7819,7 +7819,7 @@
         <v>276</v>
       </c>
       <c r="D247">
-        <v>1243</v>
+        <v>2196</v>
       </c>
       <c r="E247" t="s">
         <v>502</v>
@@ -7845,7 +7845,7 @@
         <v>269</v>
       </c>
       <c r="D248">
-        <v>254</v>
+        <v>324</v>
       </c>
       <c r="E248" t="s">
         <v>503</v>
@@ -7871,7 +7871,7 @@
         <v>274</v>
       </c>
       <c r="D249">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E249" t="s">
         <v>504</v>
@@ -7891,7 +7891,7 @@
         <v>269</v>
       </c>
       <c r="D250">
-        <v>194</v>
+        <v>356</v>
       </c>
       <c r="E250" t="s">
         <v>505</v>
@@ -7917,7 +7917,7 @@
         <v>287</v>
       </c>
       <c r="D251">
-        <v>153</v>
+        <v>240</v>
       </c>
       <c r="E251" t="s">
         <v>506</v>
@@ -7937,7 +7937,7 @@
         <v>268</v>
       </c>
       <c r="D252">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="E252" t="s">
         <v>442</v>
@@ -7957,7 +7957,7 @@
         <v>268</v>
       </c>
       <c r="D253">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="E253" t="s">
         <v>433</v>
@@ -7977,7 +7977,7 @@
         <v>268</v>
       </c>
       <c r="D254">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E254" t="s">
         <v>507</v>
@@ -8003,7 +8003,7 @@
         <v>271</v>
       </c>
       <c r="D255">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E255" t="s">
         <v>305</v>

</xml_diff>